<commit_message>
Add folders and Data files that need to be added.
</commit_message>
<xml_diff>
--- a/Data/D&C Chronological Order.xlsx
+++ b/Data/D&C Chronological Order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\R_Projects\goody\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Projects\goody\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A33758-78B9-4775-A830-6940F274ADAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0021C71-BBCF-4D23-858C-B90D74CF38DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{99A48E23-245A-48C2-952E-A6FF30C06388}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="55">
   <si>
     <t>Year</t>
   </si>
@@ -94,6 +94,111 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Kirtland</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Zion, Jackson County</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Independence</t>
+  </si>
+  <si>
+    <t>Missouri River</t>
+  </si>
+  <si>
+    <t>Chariton</t>
+  </si>
+  <si>
+    <t>Hiram</t>
+  </si>
+  <si>
+    <t>Amherst</t>
+  </si>
+  <si>
+    <t>Perrysburg</t>
+  </si>
+  <si>
+    <t>Fishing River</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Far West</t>
+  </si>
+  <si>
+    <t>Spring Hill, Daviess County</t>
+  </si>
+  <si>
+    <t>Liberty Jail, Clay County</t>
+  </si>
+  <si>
+    <t>Nauvoo</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Ramus</t>
+  </si>
+  <si>
+    <t>Winter Quarters</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Salt Lake City</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Brigham Young</t>
+  </si>
+  <si>
+    <t>Joseph F. Smith</t>
+  </si>
+  <si>
+    <t>General Assembly</t>
+  </si>
+  <si>
+    <t>Joseph Smith</t>
+  </si>
+  <si>
+    <t>Announcement</t>
+  </si>
+  <si>
+    <t>Given Too</t>
   </si>
 </sst>
 </file>
@@ -451,22 +556,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D875A20-E03E-4CA9-BDD3-2D8E08D44F66}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A24"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +591,11 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1823</v>
       </c>
@@ -505,8 +614,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1824</v>
       </c>
@@ -525,8 +637,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1829</v>
       </c>
@@ -545,8 +660,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1829</v>
       </c>
@@ -565,8 +683,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1829</v>
       </c>
@@ -585,8 +706,11 @@
       <c r="F6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1829</v>
       </c>
@@ -605,8 +729,11 @@
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1829</v>
       </c>
@@ -625,8 +752,11 @@
       <c r="F8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1829</v>
       </c>
@@ -645,8 +775,11 @@
       <c r="F9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1829</v>
       </c>
@@ -665,8 +798,11 @@
       <c r="F10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1829</v>
       </c>
@@ -685,8 +821,11 @@
       <c r="F11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1829</v>
       </c>
@@ -705,8 +844,11 @@
       <c r="F12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1829</v>
       </c>
@@ -725,8 +867,11 @@
       <c r="F13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1829</v>
       </c>
@@ -745,8 +890,11 @@
       <c r="F14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1829</v>
       </c>
@@ -765,8 +913,11 @@
       <c r="F15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1829</v>
       </c>
@@ -785,8 +936,11 @@
       <c r="F16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1829</v>
       </c>
@@ -805,8 +959,11 @@
       <c r="F17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1829</v>
       </c>
@@ -825,8 +982,11 @@
       <c r="F18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1829</v>
       </c>
@@ -845,8 +1005,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1830</v>
       </c>
@@ -865,8 +1028,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1830</v>
       </c>
@@ -885,8 +1051,11 @@
       <c r="F21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1830</v>
       </c>
@@ -905,8 +1074,11 @@
       <c r="F22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1830</v>
       </c>
@@ -925,8 +1097,11 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1830</v>
       </c>
@@ -944,6 +1119,2654 @@
       </c>
       <c r="F24">
         <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1830</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1830</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1830</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1830</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1830</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1830</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1830</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1830</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1830</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1830</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1830</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1830</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1830</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>36</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1830</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>37</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1831</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1831</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>39</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1831</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1831</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42">
+        <v>41</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1831</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43">
+        <v>42</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1831</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44">
+        <v>43</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1831</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45">
+        <v>44</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1831</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46">
+        <v>45</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1831</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47">
+        <v>46</v>
+      </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1831</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48">
+        <v>47</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1831</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49">
+        <v>48</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1831</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50">
+        <v>49</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1831</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51">
+        <v>50</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1831</v>
+      </c>
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52">
+        <v>51</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1831</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53">
+        <v>52</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1831</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54">
+        <v>53</v>
+      </c>
+      <c r="F54">
+        <v>5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1831</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55">
+        <v>54</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1831</v>
+      </c>
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>55</v>
+      </c>
+      <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1831</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57">
+        <v>56</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1831</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58">
+        <v>57</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1831</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59">
+        <v>58</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1831</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60">
+        <v>59</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1831</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61">
+        <v>60</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1831</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62">
+        <v>61</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1831</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63">
+        <v>62</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1831</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64">
+        <v>63</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1831</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65">
+        <v>64</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1831</v>
+      </c>
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66">
+        <v>65</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1831</v>
+      </c>
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67">
+        <v>66</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1831</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>6</v>
+      </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1831</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69">
+        <v>67</v>
+      </c>
+      <c r="F69">
+        <v>6</v>
+      </c>
+      <c r="G69" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1831</v>
+      </c>
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70">
+        <v>68</v>
+      </c>
+      <c r="F70">
+        <v>6</v>
+      </c>
+      <c r="G70" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1831</v>
+      </c>
+      <c r="B71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71">
+        <v>69</v>
+      </c>
+      <c r="F71">
+        <v>6</v>
+      </c>
+      <c r="G71" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1831</v>
+      </c>
+      <c r="B72" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72">
+        <v>70</v>
+      </c>
+      <c r="F72">
+        <v>6</v>
+      </c>
+      <c r="G72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1831</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73">
+        <v>133</v>
+      </c>
+      <c r="F73">
+        <v>6</v>
+      </c>
+      <c r="G73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1831</v>
+      </c>
+      <c r="B74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74">
+        <v>71</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1831</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75">
+        <v>72</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1832</v>
+      </c>
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" t="s">
+        <v>26</v>
+      </c>
+      <c r="E76">
+        <v>73</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1832</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>34</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77">
+        <v>75</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1832</v>
+      </c>
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E78">
+        <v>76</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1832</v>
+      </c>
+      <c r="B79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79">
+        <v>77</v>
+      </c>
+      <c r="F79">
+        <v>4</v>
+      </c>
+      <c r="G79" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1832</v>
+      </c>
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80">
+        <v>79</v>
+      </c>
+      <c r="F80">
+        <v>4</v>
+      </c>
+      <c r="G80" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1832</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81">
+        <v>80</v>
+      </c>
+      <c r="F81">
+        <v>4</v>
+      </c>
+      <c r="G81" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1832</v>
+      </c>
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82">
+        <v>81</v>
+      </c>
+      <c r="F82">
+        <v>4</v>
+      </c>
+      <c r="G82" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1832</v>
+      </c>
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83">
+        <v>78</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1832</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" t="s">
+        <v>29</v>
+      </c>
+      <c r="E84">
+        <v>82</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1832</v>
+      </c>
+      <c r="B85" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" t="s">
+        <v>30</v>
+      </c>
+      <c r="D85" t="s">
+        <v>29</v>
+      </c>
+      <c r="E85">
+        <v>83</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1832</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86">
+        <v>99</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1832</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87">
+        <v>84</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1832</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>25</v>
+      </c>
+      <c r="D88" t="s">
+        <v>26</v>
+      </c>
+      <c r="E88">
+        <v>85</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1832</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89" t="s">
+        <v>26</v>
+      </c>
+      <c r="E89">
+        <v>86</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1832</v>
+      </c>
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" t="s">
+        <v>25</v>
+      </c>
+      <c r="D90" t="s">
+        <v>26</v>
+      </c>
+      <c r="E90">
+        <v>87</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1832</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>25</v>
+      </c>
+      <c r="D91" t="s">
+        <v>26</v>
+      </c>
+      <c r="E91">
+        <v>88</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1833</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92">
+        <v>89</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1833</v>
+      </c>
+      <c r="B93" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" t="s">
+        <v>26</v>
+      </c>
+      <c r="E93">
+        <v>90</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1833</v>
+      </c>
+      <c r="B94" t="s">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" t="s">
+        <v>26</v>
+      </c>
+      <c r="E94">
+        <v>91</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1833</v>
+      </c>
+      <c r="B95" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" t="s">
+        <v>25</v>
+      </c>
+      <c r="D95" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95">
+        <v>92</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1833</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>25</v>
+      </c>
+      <c r="D96" t="s">
+        <v>26</v>
+      </c>
+      <c r="E96">
+        <v>93</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1833</v>
+      </c>
+      <c r="B97" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" t="s">
+        <v>26</v>
+      </c>
+      <c r="E97">
+        <v>95</v>
+      </c>
+      <c r="F97">
+        <v>2</v>
+      </c>
+      <c r="G97" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1833</v>
+      </c>
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" t="s">
+        <v>25</v>
+      </c>
+      <c r="D98" t="s">
+        <v>26</v>
+      </c>
+      <c r="E98">
+        <v>96</v>
+      </c>
+      <c r="F98">
+        <v>2</v>
+      </c>
+      <c r="G98" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1833</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" t="s">
+        <v>25</v>
+      </c>
+      <c r="D99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99">
+        <v>94</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1833</v>
+      </c>
+      <c r="B100" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" t="s">
+        <v>25</v>
+      </c>
+      <c r="D100" t="s">
+        <v>26</v>
+      </c>
+      <c r="E100">
+        <v>97</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1833</v>
+      </c>
+      <c r="B101" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" t="s">
+        <v>25</v>
+      </c>
+      <c r="D101" t="s">
+        <v>26</v>
+      </c>
+      <c r="E101">
+        <v>98</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1833</v>
+      </c>
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102">
+        <v>100</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1833</v>
+      </c>
+      <c r="B103" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" t="s">
+        <v>25</v>
+      </c>
+      <c r="D103" t="s">
+        <v>26</v>
+      </c>
+      <c r="E103">
+        <v>101</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1834</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>25</v>
+      </c>
+      <c r="D104" t="s">
+        <v>26</v>
+      </c>
+      <c r="E104">
+        <v>102</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1834</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105" t="s">
+        <v>26</v>
+      </c>
+      <c r="E105">
+        <v>103</v>
+      </c>
+      <c r="F105">
+        <v>2</v>
+      </c>
+      <c r="G105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1834</v>
+      </c>
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>25</v>
+      </c>
+      <c r="D106" t="s">
+        <v>26</v>
+      </c>
+      <c r="E106">
+        <v>104</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+      <c r="G106" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1834</v>
+      </c>
+      <c r="B107" t="s">
+        <v>16</v>
+      </c>
+      <c r="C107" t="s">
+        <v>36</v>
+      </c>
+      <c r="D107" t="s">
+        <v>29</v>
+      </c>
+      <c r="E107">
+        <v>105</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1834</v>
+      </c>
+      <c r="B108" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" t="s">
+        <v>25</v>
+      </c>
+      <c r="D108" t="s">
+        <v>26</v>
+      </c>
+      <c r="E108">
+        <v>106</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1835</v>
+      </c>
+      <c r="B109" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109" t="s">
+        <v>25</v>
+      </c>
+      <c r="D109" t="s">
+        <v>26</v>
+      </c>
+      <c r="E109">
+        <v>107</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+      <c r="G109" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1835</v>
+      </c>
+      <c r="B110" t="s">
+        <v>20</v>
+      </c>
+      <c r="C110" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110" t="s">
+        <v>26</v>
+      </c>
+      <c r="E110">
+        <v>134</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1835</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" t="s">
+        <v>25</v>
+      </c>
+      <c r="D111" t="s">
+        <v>26</v>
+      </c>
+      <c r="E111">
+        <v>108</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1836</v>
+      </c>
+      <c r="B112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" t="s">
+        <v>26</v>
+      </c>
+      <c r="E112">
+        <v>137</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1836</v>
+      </c>
+      <c r="B113" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" t="s">
+        <v>25</v>
+      </c>
+      <c r="D113" t="s">
+        <v>26</v>
+      </c>
+      <c r="E113">
+        <v>109</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="G113" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1836</v>
+      </c>
+      <c r="B114" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114">
+        <v>110</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1836</v>
+      </c>
+      <c r="B115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D115" t="s">
+        <v>38</v>
+      </c>
+      <c r="E115">
+        <v>111</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1837</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116" t="s">
+        <v>26</v>
+      </c>
+      <c r="E116">
+        <v>112</v>
+      </c>
+      <c r="F116">
+        <v>1</v>
+      </c>
+      <c r="G116" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1838</v>
+      </c>
+      <c r="B117" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>29</v>
+      </c>
+      <c r="E117">
+        <v>113</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+      <c r="G117" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1838</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" t="s">
+        <v>29</v>
+      </c>
+      <c r="E118">
+        <v>114</v>
+      </c>
+      <c r="F118">
+        <v>2</v>
+      </c>
+      <c r="G118" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1838</v>
+      </c>
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119">
+        <v>115</v>
+      </c>
+      <c r="F119">
+        <v>2</v>
+      </c>
+      <c r="G119" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1838</v>
+      </c>
+      <c r="B120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>40</v>
+      </c>
+      <c r="D120" t="s">
+        <v>29</v>
+      </c>
+      <c r="E120">
+        <v>116</v>
+      </c>
+      <c r="F120">
+        <v>1</v>
+      </c>
+      <c r="G120" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1838</v>
+      </c>
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" t="s">
+        <v>29</v>
+      </c>
+      <c r="E121">
+        <v>117</v>
+      </c>
+      <c r="F121">
+        <v>4</v>
+      </c>
+      <c r="G121" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1838</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" t="s">
+        <v>29</v>
+      </c>
+      <c r="E122">
+        <v>118</v>
+      </c>
+      <c r="F122">
+        <v>4</v>
+      </c>
+      <c r="G122" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1838</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" t="s">
+        <v>29</v>
+      </c>
+      <c r="E123">
+        <v>119</v>
+      </c>
+      <c r="F123">
+        <v>4</v>
+      </c>
+      <c r="G123" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1838</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" t="s">
+        <v>29</v>
+      </c>
+      <c r="E124">
+        <v>120</v>
+      </c>
+      <c r="F124">
+        <v>4</v>
+      </c>
+      <c r="G124" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1839</v>
+      </c>
+      <c r="B125" t="s">
+        <v>13</v>
+      </c>
+      <c r="C125" t="s">
+        <v>41</v>
+      </c>
+      <c r="D125" t="s">
+        <v>29</v>
+      </c>
+      <c r="E125">
+        <v>121</v>
+      </c>
+      <c r="F125">
+        <v>3</v>
+      </c>
+      <c r="G125" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1839</v>
+      </c>
+      <c r="B126" t="s">
+        <v>13</v>
+      </c>
+      <c r="C126" t="s">
+        <v>41</v>
+      </c>
+      <c r="D126" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126">
+        <v>122</v>
+      </c>
+      <c r="F126">
+        <v>3</v>
+      </c>
+      <c r="G126" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1839</v>
+      </c>
+      <c r="B127" t="s">
+        <v>13</v>
+      </c>
+      <c r="C127" t="s">
+        <v>41</v>
+      </c>
+      <c r="D127" t="s">
+        <v>29</v>
+      </c>
+      <c r="E127">
+        <v>123</v>
+      </c>
+      <c r="F127">
+        <v>3</v>
+      </c>
+      <c r="G127" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1841</v>
+      </c>
+      <c r="B128" t="s">
+        <v>24</v>
+      </c>
+      <c r="C128" t="s">
+        <v>42</v>
+      </c>
+      <c r="D128" t="s">
+        <v>43</v>
+      </c>
+      <c r="E128">
+        <v>124</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1841</v>
+      </c>
+      <c r="B129" t="s">
+        <v>13</v>
+      </c>
+      <c r="C129" t="s">
+        <v>42</v>
+      </c>
+      <c r="D129" t="s">
+        <v>43</v>
+      </c>
+      <c r="E129">
+        <v>125</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>1841</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>42</v>
+      </c>
+      <c r="D130" t="s">
+        <v>43</v>
+      </c>
+      <c r="E130">
+        <v>126</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1842</v>
+      </c>
+      <c r="B131" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" t="s">
+        <v>42</v>
+      </c>
+      <c r="D131" t="s">
+        <v>43</v>
+      </c>
+      <c r="E131">
+        <v>127</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="G131" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>1842</v>
+      </c>
+      <c r="B132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" t="s">
+        <v>42</v>
+      </c>
+      <c r="D132" t="s">
+        <v>43</v>
+      </c>
+      <c r="E132">
+        <v>128</v>
+      </c>
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="G132" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1843</v>
+      </c>
+      <c r="B133" t="s">
+        <v>12</v>
+      </c>
+      <c r="C133" t="s">
+        <v>42</v>
+      </c>
+      <c r="D133" t="s">
+        <v>43</v>
+      </c>
+      <c r="E133">
+        <v>129</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="G133" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>1843</v>
+      </c>
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134" t="s">
+        <v>44</v>
+      </c>
+      <c r="D134" t="s">
+        <v>43</v>
+      </c>
+      <c r="E134">
+        <v>130</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1843</v>
+      </c>
+      <c r="B135" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" t="s">
+        <v>44</v>
+      </c>
+      <c r="D135" t="s">
+        <v>43</v>
+      </c>
+      <c r="E135">
+        <v>131</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="G135" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>1843</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" t="s">
+        <v>42</v>
+      </c>
+      <c r="D136" t="s">
+        <v>43</v>
+      </c>
+      <c r="E136">
+        <v>132</v>
+      </c>
+      <c r="F136">
+        <v>1</v>
+      </c>
+      <c r="G136" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1844</v>
+      </c>
+      <c r="B137" t="s">
+        <v>16</v>
+      </c>
+      <c r="C137" t="s">
+        <v>42</v>
+      </c>
+      <c r="D137" t="s">
+        <v>43</v>
+      </c>
+      <c r="E137">
+        <v>135</v>
+      </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="G137" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1847</v>
+      </c>
+      <c r="B138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" t="s">
+        <v>45</v>
+      </c>
+      <c r="D138" t="s">
+        <v>46</v>
+      </c>
+      <c r="E138">
+        <v>136</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1918</v>
+      </c>
+      <c r="B139" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" t="s">
+        <v>47</v>
+      </c>
+      <c r="D139" t="s">
+        <v>48</v>
+      </c>
+      <c r="E139">
+        <v>138</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
+      <c r="G139" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>